<commit_message>
Update design. -Update documents of design.
</commit_message>
<xml_diff>
--- a/dev/doc/view_model_archi_design.xlsx
+++ b/dev/doc/view_model_archi_design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>○</t>
     <phoneticPr fontId="2"/>
@@ -78,66 +78,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>前輪の回転数</t>
-    <rPh sb="0" eb="2">
-      <t>ゼンリン</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>カイテンスウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>前輪の速度</t>
-    <rPh sb="0" eb="2">
-      <t>ゼンリン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ソクド</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>後輪の回転数</t>
-    <rPh sb="0" eb="2">
-      <t>コウリン</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>カイテンスウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>後輪の速度</t>
-    <rPh sb="0" eb="2">
-      <t>コウリン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ソクド</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>車体の回転数</t>
-    <rPh sb="0" eb="2">
-      <t>シャタイ</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>カイテンスウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>車体の速度</t>
-    <rPh sb="0" eb="2">
-      <t>シャタイ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ソクド</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>備考：</t>
     <rPh sb="0" eb="2">
       <t>ビコウ</t>
@@ -174,6 +114,96 @@
     <rPh sb="14" eb="17">
       <t>ヘイキンチ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>前輪の回転数(生値)</t>
+    <rPh sb="0" eb="2">
+      <t>ゼンリン</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カイテンスウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ナマ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>前輪の速度(生値)</t>
+    <rPh sb="0" eb="2">
+      <t>ゼンリン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ソクド</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>後輪の回転数(生値)</t>
+    <rPh sb="0" eb="2">
+      <t>コウリン</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カイテンスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>後輪の速度(生値)</t>
+    <rPh sb="0" eb="2">
+      <t>コウリン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ソクド</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>車体の回転数(生値)</t>
+    <rPh sb="0" eb="2">
+      <t>シャタイ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カイテンスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>車体の速度(生値)</t>
+    <rPh sb="0" eb="2">
+      <t>シャタイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ソクド</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>車体の回転数(表示値)</t>
+    <rPh sb="0" eb="2">
+      <t>シャタイ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カイテンスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>車体の速度(表示値)</t>
+    <rPh sb="0" eb="2">
+      <t>シャタイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ソクド</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -234,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -502,11 +532,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -589,10 +679,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1133,8 +1238,8 @@
       <xdr:rowOff>102288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>102288</xdr:rowOff>
     </xdr:to>
@@ -1277,8 +1382,8 @@
       <xdr:rowOff>143700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>143700</xdr:rowOff>
     </xdr:to>
@@ -1956,7 +2061,7 @@
   <dimension ref="C2:N35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ31" sqref="AQ31"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1966,8 +2071,9 @@
     <col min="6" max="6" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="2" style="1"/>
+    <col min="9" max="9" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="2" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.15">
@@ -1983,7 +2089,7 @@
       <c r="D3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2032,7 +2138,7 @@
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="F9" s="13" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.15">
@@ -2042,11 +2148,11 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C11" s="13"/>
@@ -2055,11 +2161,11 @@
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
-      <c r="N11" s="25"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C12" s="13"/>
@@ -2068,11 +2174,11 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
+      <c r="J12" s="23"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
+      <c r="N12" s="24"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C13" s="13"/>
@@ -2081,11 +2187,11 @@
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C14" s="13"/>
@@ -2094,11 +2200,11 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="J14" s="23"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C15" s="13"/>
@@ -2107,11 +2213,11 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
+      <c r="N15" s="24"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C16" s="13"/>
@@ -2120,11 +2226,11 @@
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
+      <c r="N16" s="24"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C17" s="13"/>
@@ -2133,11 +2239,11 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
-      <c r="N17" s="25"/>
+      <c r="N17" s="24"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C18" s="13"/>
@@ -2146,11 +2252,11 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
+      <c r="J18" s="23"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
+      <c r="N18" s="24"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C19" s="13"/>
@@ -2159,11 +2265,11 @@
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="J19" s="23"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
+      <c r="N19" s="24"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C20" s="13"/>
@@ -2172,11 +2278,11 @@
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
+      <c r="J20" s="23"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
+      <c r="N20" s="24"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C21" s="13"/>
@@ -2185,11 +2291,11 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
+      <c r="N21" s="24"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C22" s="13"/>
@@ -2198,11 +2304,11 @@
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
+      <c r="J22" s="23"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
+      <c r="N22" s="24"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C23" s="13"/>
@@ -2211,11 +2317,11 @@
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
+      <c r="J23" s="23"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
-      <c r="N23" s="25"/>
+      <c r="N23" s="24"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C24" s="13"/>
@@ -2224,11 +2330,11 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="14"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.15">
       <c r="C25" s="13"/>
@@ -2239,7 +2345,7 @@
       <c r="D26" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="28" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2249,8 +2355,14 @@
       <c r="G27" s="8">
         <v>0</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="31">
         <v>1</v>
+      </c>
+      <c r="I27" s="31">
+        <v>2</v>
+      </c>
+      <c r="J27" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.15">
@@ -2260,10 +2372,16 @@
         <v>0</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.15">
@@ -2273,10 +2391,16 @@
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H29" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="3:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -2286,10 +2410,16 @@
         <v>2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.15">
@@ -2297,36 +2427,38 @@
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.15">
-      <c r="F32" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="F32" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="21"/>
+      <c r="H32" s="22"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.15">
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="22"/>
+      <c r="G33" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="25"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.15">
       <c r="F34" s="23"/>
       <c r="G34" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="H34" s="25"/>
       <c r="I34" s="24"/>
-      <c r="J34" s="25"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.15">
       <c r="F35" s="26"/>
       <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>